<commit_message>
fix(wasm): preserve modern Excel errors on XLSX import
- Ensure XLSX-imported ErrorValue::{Field,Connect,Blocked,Unknown} stay real engine errors (so ISERROR behaves like Excel).
- Extend bool-error.xlsx fixture + generator with modern error literals and add wasm-bindgen regression test.
- Fix compilation issues introduced by recent rich-value/rich-data changes (cellimages module collision, rich-data helper dupes, VBA signature OID parsing).
</commit_message>
<xml_diff>
--- a/fixtures/xlsx/basic/bool-error.xlsx
+++ b/fixtures/xlsx/basic/bool-error.xlsx
@@ -59,6 +59,18 @@
       <c r="B1" t="e">
         <v>#DIV/0!</v>
       </c>
+      <c r="C1" t="e">
+        <v>#FIELD!</v>
+      </c>
+      <c r="D1" t="e">
+        <v>#CONNECT!</v>
+      </c>
+      <c r="E1" t="e">
+        <v>#BLOCKED!</v>
+      </c>
+      <c r="F1" t="e">
+        <v>#UNKNOWN!</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="b">

</xml_diff>